<commit_message>
update anh tuan nb + lapdat
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/1.NhanBH/NBH221115_AnhTuanNB.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/1.NhanBH/NBH221115_AnhTuanNB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t xml:space="preserve">STT </t>
   </si>
@@ -520,6 +520,54 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -546,54 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +951,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -968,92 +968,92 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="52"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
@@ -1076,126 +1076,130 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="30">
         <v>1</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54" t="s">
+      <c r="D11" s="31"/>
+      <c r="E11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
+      <c r="A12" s="30">
         <v>2</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="54"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53">
+      <c r="A13" s="30">
         <v>3</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="54"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="30">
         <v>4</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54" t="s">
+      <c r="D14" s="31"/>
+      <c r="E14" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="54"/>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53">
+      <c r="A15" s="30">
         <v>5</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54" t="s">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="54"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53">
+      <c r="A16" s="30">
         <v>6</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
+      <c r="A17" s="30">
         <v>7</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
+      <c r="A18" s="30">
         <v>8</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
@@ -1209,23 +1213,23 @@
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42" t="s">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="47"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
@@ -1261,16 +1265,16 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41" t="s">
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="48"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="41"/>
     </row>
     <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
@@ -1298,6 +1302,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="B21:C21"/>
@@ -1307,11 +1316,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>